<commit_message>
- "Append current year" DEFAULT Checked - Warning in caso di anni non correnti presenti (solo in modalità append)-Zip del file backup - "Attendere prego" in frmMain
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Superdettagli.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Superdettagli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3718B5F8-175D-4401-977D-F3E5968D5B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E961B0CD-5696-4161-ADD7-5E4A850DAA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:CL7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2008,7 @@
         <v>127</v>
       </c>
       <c r="AE4">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="AF4" t="s">
         <v>128</v>

</xml_diff>